<commit_message>
Se agrega vista Enviar Acuerdos
</commit_message>
<xml_diff>
--- a/asset/production/uploads/solicitud.xlsx
+++ b/asset/production/uploads/solicitud.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Javier_Toto\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jafernandez\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94DF39C-C5D6-4775-9421-6797B76566B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7695" tabRatio="993"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7695" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formato" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>TIPO DOCUMENTO</t>
   </si>
@@ -69,19 +70,34 @@
     <t>NIT EMPRESA</t>
   </si>
   <si>
-    <t>Javier Augusto</t>
-  </si>
-  <si>
-    <t>Fernández</t>
-  </si>
-  <si>
-    <t>totojavi81@hotmail.com</t>
+    <t>Lili</t>
+  </si>
+  <si>
+    <t>Llanos</t>
+  </si>
+  <si>
+    <t>lili@gmail.com</t>
+  </si>
+  <si>
+    <t>Axede</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h@hotmail.com</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4">
     <font>
       <sz val="10"/>
@@ -191,7 +207,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -537,11 +553,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -597,7 +613,7 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>80239379</v>
+        <v>53071568</v>
       </c>
       <c r="D2" t="s">
         <v>14</v>
@@ -609,15 +625,54 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>3046200176</v>
+        <v>3013109613</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2">
+        <v>8179562531</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>9846</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3">
+        <v>2565855</v>
+      </c>
+      <c r="G3">
+        <v>301232562</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3">
+        <v>66616161661</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{5062F316-0D33-4F8F-B6E2-ACC50BA0C603}"/>
+    <hyperlink ref="H3" r:id="rId2" xr:uid="{32C597E2-430D-4F24-A53A-D88713DA787C}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -629,7 +684,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>

</xml_diff>